<commit_message>
November 24, 2021 first commit
</commit_message>
<xml_diff>
--- a/e-University_Database_Project/DBMD University Project Sample Data.xlsx
+++ b/e-University_Database_Project/DBMD University Project Sample Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/intuition/Desktop/e-University Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/intuition/Desktop/GITHUB/data_analysis_and_data_visualization_projects/e-University_Database_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70985113-EC4B-E648-9BED-F74BC5C0DB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2C84F9-4983-C040-B96C-694504E7DB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -638,23 +638,27 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="24.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" customWidth="1"/>
-    <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5" customWidth="1"/>
-    <col min="14" max="15" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="19.33203125" bestFit="1" customWidth="1"/>

</xml_diff>